<commit_message>
Samling af pointberegning med bonus og slutspil
</commit_message>
<xml_diff>
--- a/Slutspil.xlsx
+++ b/Slutspil.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gustav/Desktop/TBTFEuro-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6E9640-5B1B-4242-A2AA-282D714E15E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0148048E-E52F-9144-A030-EC80A757BE41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0C23152F-2A27-D043-AACC-C0BBA788D8AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{0C23152F-2A27-D043-AACC-C0BBA788D8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -481,7 +481,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="C2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -519,12 +519,6 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -533,12 +527,6 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -547,12 +535,6 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -561,12 +543,6 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -575,12 +551,6 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -589,12 +559,6 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -603,12 +567,6 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -617,51 +575,45 @@
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f>IF(C2="","",IF(C2&gt;D2,A2,IF(D2&gt;C2,B2,IF(E2&gt;F2,A2,IF(F2&gt;E2,B2,IF(G2&gt;H2,A2,IF(H2&gt;G2,B2,"")))))))</f>
-        <v>Spanien</v>
+        <v/>
       </c>
       <c r="B10" t="str">
         <f>IF(C3="","",IF(C3&gt;D3,A3,IF(D3&gt;C3,B3,IF(E3&gt;F3,A3,IF(F3&gt;E3,B3,IF(G3&gt;H3,A3,IF(H3&gt;G3,B3,"")))))))</f>
-        <v>Danmark</v>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f>IF(C4="","",IF(C4&gt;D4,A4,IF(D4&gt;C4,B4,IF(E4&gt;F4,A4,IF(F4&gt;E4,B4,IF(G4&gt;H4,A4,IF(H4&gt;G4,B4,"")))))))</f>
-        <v>Portugal</v>
+        <v/>
       </c>
       <c r="B11" t="str">
         <f>IF(C5="","",IF(C5&gt;D5,A5,IF(D5&gt;C5,B5,IF(E5&gt;F5,A5,IF(F5&gt;E5,B5,IF(G5&gt;H5,A5,IF(H5&gt;G5,B5,"")))))))</f>
-        <v>Frankrig</v>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f>IF(C6="","",IF(C6&gt;D6,A6,IF(D6&gt;C6,B6,IF(E6&gt;F6,A6,IF(F6&gt;E6,B6,IF(G6&gt;H6,A6,IF(H6&gt;G6,B6,"")))))))</f>
-        <v>Holland</v>
+        <v/>
       </c>
       <c r="B12" t="str">
         <f>IF(C7="","",IF(C7&gt;D7,A7,IF(D7&gt;C7,B7,IF(E7&gt;F7,A7,IF(F7&gt;E7,B7,IF(G7&gt;H7,A7,IF(H7&gt;G7,B7,"")))))))</f>
-        <v>Østrig</v>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f>IF(C8="","",IF(C8&gt;D8,A8,IF(D8&gt;C8,B8,IF(E8&gt;F8,A8,IF(F8&gt;E8,B8,IF(G8&gt;H8,A8,IF(H8&gt;G8,B8,"")))))))</f>
-        <v>Slovakiet</v>
+        <v/>
       </c>
       <c r="B13" t="str">
         <f>IF(C9="","",IF(C9&gt;D9,A9,IF(D9&gt;C9,B9,IF(E9&gt;F9,A9,IF(F9&gt;E9,B9,IF(G9&gt;H9,A9,IF(H9&gt;G9,B9,"")))))))</f>
-        <v>Schweiz</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>